<commit_message>
checkpoint * implement pascal and camel case converts. * modify DataType spec
</commit_message>
<xml_diff>
--- a/Code/Tests/Tests.Daterpillar/data.xlsx
+++ b/Code/Tests/Tests.Daterpillar/data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +18,100 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>PASCAL</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Title Case</t>
+  </si>
+  <si>
+    <t>TitleCase</t>
+  </si>
+  <si>
+    <t>Mixed Case</t>
+  </si>
+  <si>
+    <t>camelCase</t>
+  </si>
+  <si>
+    <t>Camelcase</t>
+  </si>
+  <si>
+    <t>CamelCase</t>
+  </si>
+  <si>
+    <t>PascalCase</t>
+  </si>
+  <si>
+    <t>Pascalcase</t>
+  </si>
+  <si>
+    <t>MiXedCaSE</t>
+  </si>
+  <si>
+    <t>miXed caSE</t>
+  </si>
+  <si>
+    <t>lower case</t>
+  </si>
+  <si>
+    <t>Lower Case</t>
+  </si>
+  <si>
+    <t>LowerCase</t>
+  </si>
+  <si>
+    <t>UPPER CASE</t>
+  </si>
+  <si>
+    <t>UPPERCASE</t>
+  </si>
+  <si>
+    <t>Upper Case</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>CAMEL</t>
+  </si>
+  <si>
+    <t>titleCase</t>
+  </si>
+  <si>
+    <t>pascalCase</t>
+  </si>
+  <si>
+    <t>lowerCase</t>
+  </si>
+  <si>
+    <t>uPPERCASE</t>
+  </si>
+  <si>
+    <t>miXedCaSE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,6 +160,19 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="TEXT"/>
+    <tableColumn id="4" name="CAMEL"/>
+    <tableColumn id="3" name="PASCAL"/>
+    <tableColumn id="2" name="TITLE"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -111,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -146,7 +251,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -323,7 +428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -331,12 +436,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* complete integration testing of SQLiteTemplate
</commit_message>
<xml_diff>
--- a/Code/Tests/Tests.Daterpillar/data.xlsx
+++ b/Code/Tests/Tests.Daterpillar/data.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
+    <sheet name="DataTypes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>TEXT</t>
   </si>
@@ -106,12 +107,126 @@
   </si>
   <si>
     <t>miXedCaSE</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>bigInt</t>
+  </si>
+  <si>
+    <t>mediumInt</t>
+  </si>
+  <si>
+    <t>smallInt</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>T-SQL</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>sbyte</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Timespan</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>BLOB</t>
+  </si>
+  <si>
+    <t>CHAR</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>BIGINT</t>
+  </si>
+  <si>
+    <t>VARCHAR(0)</t>
+  </si>
+  <si>
+    <t>DECIMAL(0, 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,7 +284,21 @@
     <tableColumn id="3" name="PASCAL"/>
     <tableColumn id="2" name="TITLE"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E16" totalsRowShown="0">
+  <autoFilter ref="A1:E16"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Type"/>
+    <tableColumn id="5" name="C#"/>
+    <tableColumn id="3" name="MySQL"/>
+    <tableColumn id="2" name="SQLite"/>
+    <tableColumn id="4" name="T-SQL"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -216,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -251,7 +380,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -428,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,18 +567,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -477,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -491,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -505,7 +634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -519,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -533,7 +662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -547,7 +676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -561,7 +690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -581,4 +710,212 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implement and partilly test CSharpTemplate
</commit_message>
<xml_diff>
--- a/Code/Tests/Tests.Daterpillar/data.xlsx
+++ b/Code/Tests/Tests.Daterpillar/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>TEXT</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>DateTime</t>
-  </si>
-  <si>
-    <t>Timespan</t>
   </si>
   <si>
     <t>Type</t>
@@ -717,7 +714,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,7 +728,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
@@ -754,7 +751,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -765,7 +762,7 @@
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -776,7 +773,7 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -798,7 +795,7 @@
         <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -809,7 +806,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -820,7 +817,7 @@
         <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -831,7 +828,7 @@
         <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -842,7 +839,7 @@
         <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -853,7 +850,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -864,7 +861,7 @@
         <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -875,7 +872,7 @@
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -886,7 +883,7 @@
         <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -894,10 +891,10 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -908,7 +905,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* validate c# code with roslyn. * start framework for mysql template.
</commit_message>
<xml_diff>
--- a/Code/Tests/Tests.Daterpillar/data.xlsx
+++ b/Code/Tests/Tests.Daterpillar/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>TEXT</t>
   </si>
@@ -218,12 +218,24 @@
   </si>
   <si>
     <t>DECIMAL(0, 0)</t>
+  </si>
+  <si>
+    <t>BOOL</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>MEDIUMINT</t>
+  </si>
+  <si>
+    <t>SMALLINT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -377,7 +389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -554,7 +566,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,11 +580,11 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,16 +726,15 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -750,6 +761,9 @@
       <c r="B2" t="s">
         <v>29</v>
       </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
       <c r="D2" t="s">
         <v>54</v>
       </c>
@@ -761,6 +775,9 @@
       <c r="B3" t="s">
         <v>48</v>
       </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
       <c r="D3" t="s">
         <v>55</v>
       </c>
@@ -772,6 +789,9 @@
       <c r="B4" t="s">
         <v>31</v>
       </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
       <c r="D4" t="s">
         <v>56</v>
       </c>
@@ -783,6 +803,9 @@
       <c r="B5" t="s">
         <v>48</v>
       </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -794,6 +817,9 @@
       <c r="B6" t="s">
         <v>48</v>
       </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
       <c r="D6" t="s">
         <v>64</v>
       </c>
@@ -805,6 +831,9 @@
       <c r="B7" t="s">
         <v>34</v>
       </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
       <c r="D7" t="s">
         <v>57</v>
       </c>
@@ -816,6 +845,9 @@
       <c r="B8" t="s">
         <v>49</v>
       </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
       <c r="D8" t="s">
         <v>63</v>
       </c>
@@ -827,6 +859,9 @@
       <c r="B9" t="s">
         <v>50</v>
       </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
       <c r="D9" t="s">
         <v>57</v>
       </c>
@@ -838,6 +873,9 @@
       <c r="B10" t="s">
         <v>51</v>
       </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
       <c r="D10" t="s">
         <v>57</v>
       </c>
@@ -849,6 +887,9 @@
       <c r="B11" t="s">
         <v>38</v>
       </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
       <c r="D11" t="s">
         <v>58</v>
       </c>
@@ -860,6 +901,9 @@
       <c r="B12" t="s">
         <v>39</v>
       </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
       <c r="D12" t="s">
         <v>59</v>
       </c>
@@ -871,6 +915,9 @@
       <c r="B13" t="s">
         <v>40</v>
       </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
       <c r="D13" t="s">
         <v>65</v>
       </c>
@@ -882,6 +929,9 @@
       <c r="B14" t="s">
         <v>52</v>
       </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
       <c r="D14" t="s">
         <v>60</v>
       </c>
@@ -893,6 +943,9 @@
       <c r="B15" t="s">
         <v>52</v>
       </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
       <c r="D15" t="s">
         <v>61</v>
       </c>
@@ -903,6 +956,9 @@
       </c>
       <c r="B16" t="s">
         <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
       </c>
       <c r="D16" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
* implement mysql template. * create sqlite t4 template.
</commit_message>
<xml_diff>
--- a/Code/Tests/Tests.Daterpillar/data.xlsx
+++ b/Code/Tests/Tests.Daterpillar/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>BLOB</t>
   </si>
   <si>
-    <t>CHAR</t>
-  </si>
-  <si>
     <t>INTEGER</t>
   </si>
   <si>
@@ -230,12 +227,15 @@
   </si>
   <si>
     <t>SMALLINT</t>
+  </si>
+  <si>
+    <t>CHAR(0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -566,7 +566,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -580,11 +580,11 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -726,15 +726,15 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -762,7 +762,7 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -790,10 +790,10 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -818,10 +818,10 @@
         <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -832,10 +832,10 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -846,10 +846,10 @@
         <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -860,10 +860,10 @@
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -874,10 +874,10 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -888,10 +888,10 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -902,10 +902,10 @@
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -916,10 +916,10 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -930,10 +930,10 @@
         <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -944,10 +944,10 @@
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -958,10 +958,10 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* complete integration testing of AdoNetConnectionWrapper.
</commit_message>
<xml_diff>
--- a/Code/Tests/Tests.Daterpillar/data.xlsx
+++ b/Code/Tests/Tests.Daterpillar/data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Text_Formats" sheetId="1" r:id="rId1"/>
     <sheet name="DataTypes" sheetId="2" r:id="rId2"/>
+    <sheet name="Songs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
   <si>
     <t>TEXT</t>
   </si>
@@ -230,6 +231,36 @@
   </si>
   <si>
     <t>CHAR(0)</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Album_Id</t>
+  </si>
+  <si>
+    <t>Artist_Id</t>
+  </si>
+  <si>
+    <t>Genre_Id</t>
+  </si>
+  <si>
+    <t>Folgers Crystals</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>On_Device</t>
   </si>
 </sst>
 </file>
@@ -311,6 +342,23 @@
 </table>
 </file>
 
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H4" totalsRowShown="0">
+  <autoFilter ref="A1:H4"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="3" name="Length"/>
+    <tableColumn id="4" name="Price"/>
+    <tableColumn id="5" name="Album_Id"/>
+    <tableColumn id="6" name="Artist_Id"/>
+    <tableColumn id="7" name="Genre_Id"/>
+    <tableColumn id="8" name="On_Device"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -354,7 +402,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -389,7 +437,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -725,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -971,4 +1019,121 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2">
+        <v>2.23</v>
+      </c>
+      <c r="D2">
+        <v>1.29</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3">
+        <v>26.03</v>
+      </c>
+      <c r="D3">
+        <v>9.99</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1.29</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>